<commit_message>
fix: update results analysis table
</commit_message>
<xml_diff>
--- a/results/manual_random_analysis/apiguru_manual_mismatches_random_analysis.xlsx
+++ b/results/manual_random_analysis/apiguru_manual_mismatches_random_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uqar01-my.sharepoint.com/personal/morg0037_uqar_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68C93F48-88BF-4C58-9166-DA0938FD2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5C4AF8C-A448-48D2-AEF1-204ADE4F2839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{59ADC6F6-CADE-4022-8C41-0BBDC187392D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>Api</t>
   </si>
@@ -116,6 +116,9 @@
     <t>sportsdata</t>
   </si>
   <si>
+    <t>sports</t>
+  </si>
+  <si>
     <t>sportdata</t>
   </si>
   <si>
@@ -174,6 +177,9 @@
   </si>
   <si>
     <t>furkot_auth_access_code,furkot,furkot_auth_implicit,nfurkot,trip_id,protocol,trip,passthru,walk,access_token,user,truncated,trips,step,route,rest,users,nusing,pass,providername,algorithm,applications,html</t>
+  </si>
+  <si>
+    <t>travel</t>
   </si>
   <si>
     <t>Charity API</t>
@@ -264,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,9 +302,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,8 +643,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -675,8 +688,8 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -695,8 +708,8 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -715,8 +728,8 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -755,19 +768,19 @@
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -779,15 +792,15 @@
         <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -795,22 +808,22 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>25</v>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -824,33 +837,33 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -859,35 +872,35 @@
         <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -895,8 +908,8 @@
       <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -904,70 +917,70 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -984,53 +997,53 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -1044,22 +1057,22 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1068,15 +1081,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA69B14812F64841A25A1E1DA64BABA7" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="10e31dc1b1e3e385dc3872c96a446267">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fe87c1a5-27bd-4ef9-ac77-b5feca5bb436" xmlns:ns4="030476a9-56ef-485f-afbd-c2d58ce9f7ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7338e423c0e5f5eec2cfda34429f5cd1" ns3:_="" ns4:_="">
     <xsd:import namespace="fe87c1a5-27bd-4ef9-ac77-b5feca5bb436"/>
@@ -1323,7 +1327,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="fe87c1a5-27bd-4ef9-ac77-b5feca5bb436" xsi:nil="true"/>
@@ -1331,14 +1335,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C1BD7C1-0E6F-4AD7-8E95-0CEDA8627CCC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5726356C-A7CF-4FDB-80E3-D4AC3660C41D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5726356C-A7CF-4FDB-80E3-D4AC3660C41D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B32EB044-7FAF-47B4-A3DA-D26AADB0B993}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B32EB044-7FAF-47B4-A3DA-D26AADB0B993}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C1BD7C1-0E6F-4AD7-8E95-0CEDA8627CCC}"/>
 </file>
</xml_diff>